<commit_message>
Update schedule file: Y5_B2526_General_&_Special_Internal_2_B2_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y5_B2526_General_&_Special_Internal_2_B2_schedule.xlsx
+++ b/modules_schedules/Y5_B2526_General_&_Special_Internal_2_B2_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2582,6 +2582,1441 @@
         <v>360</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E61" s="7" t="inlineStr">
+        <is>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>07/12/2025</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E65" s="7" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E66" s="3" t="inlineStr">
+        <is>
+          <t>13/12/2025</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B67" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E67" s="7" t="inlineStr">
+        <is>
+          <t>14/12/2025</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E69" s="7" t="inlineStr">
+        <is>
+          <t>16/12/2025</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>endocrinology</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="F70" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E71" s="7" t="inlineStr">
+        <is>
+          <t>20/12/2025</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E73" s="7" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G73" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>23/12/2025</t>
+        </is>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E75" s="7" t="inlineStr">
+        <is>
+          <t>24/12/2025</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>27/12/2025</t>
+        </is>
+      </c>
+      <c r="F76" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E77" s="7" t="inlineStr">
+        <is>
+          <t>28/12/2025</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E79" s="7" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>gastroenterology</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="F80" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>nephrology</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E81" s="7" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>nephrology</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>04/01/2026</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>nephrology</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E83" s="7" t="inlineStr">
+        <is>
+          <t>05/01/2026</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>nephrology</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E84" s="3" t="inlineStr">
+        <is>
+          <t>06/01/2026</t>
+        </is>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C85" s="6" t="inlineStr">
+        <is>
+          <t>nephrology</t>
+        </is>
+      </c>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E85" s="7" t="inlineStr">
+        <is>
+          <t>07/01/2026</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>17/01/2026</t>
+        </is>
+      </c>
+      <c r="F86" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G86" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B87" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C87" s="6" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D87" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E87" s="7" t="inlineStr">
+        <is>
+          <t>18/01/2026</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G88" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E89" s="7" t="inlineStr">
+        <is>
+          <t>20/01/2026</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E90" s="3" t="inlineStr">
+        <is>
+          <t>21/01/2026</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B91" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C91" s="6" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E91" s="7" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="F92" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G92" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B93" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E93" s="7" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G93" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>neurology</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>10/02/2026</t>
+        </is>
+      </c>
+      <c r="F94" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G94" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B95" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C95" s="6" t="inlineStr">
+        <is>
+          <t>physical medicine</t>
+        </is>
+      </c>
+      <c r="D95" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E95" s="7" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G95" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>physical medicine</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>11/02/2026</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G96" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B97" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>rheumatology</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E97" s="7" t="inlineStr">
+        <is>
+          <t>10/01/2026</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G97" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>rheumatology</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="F98" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G98" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B99" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C99" s="6" t="inlineStr">
+        <is>
+          <t>rheumatology</t>
+        </is>
+      </c>
+      <c r="D99" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E99" s="7" t="inlineStr">
+        <is>
+          <t>12/01/2026</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G99" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>rheumatology</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>13/01/2026</t>
+        </is>
+      </c>
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G100" s="5" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B101" s="6" t="inlineStr">
+        <is>
+          <t>B2-A2</t>
+        </is>
+      </c>
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>rheumatology</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E101" s="7" t="inlineStr">
+        <is>
+          <t>14/01/2026</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G101" s="9" t="n">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>